<commit_message>
creados flujos falsos para ajustar el gráfico
</commit_message>
<xml_diff>
--- a/1.data/nodes_dict.xlsx
+++ b/1.data/nodes_dict.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4ba23d5b7de37717/Documentos/proyectos/03_GDP_visualization/1.data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="11_F25DC773A252ABDACC104888C19C6AFE5BDE58F4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FF714DE6-8B98-440D-97A5-3B6E7ABF22AD}"/>
+  <xr:revisionPtr revIDLastSave="73" documentId="11_F25DC773A252ABDACC104888C19C6AFE5BDE58F4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9FB0C464-3031-4AAC-8D61-605A3EDA94A0}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="88">
   <si>
     <t>names</t>
   </si>
@@ -177,7 +177,118 @@
     <t>VPNdAyTC</t>
   </si>
   <si>
-    <t>Remuneración de \n los asalariados</t>
+    <t>Remun. de los asalariados</t>
+  </si>
+  <si>
+    <t>EBE / RMB</t>
+  </si>
+  <si>
+    <t>PIB</t>
+  </si>
+  <si>
+    <t>RNB</t>
+  </si>
+  <si>
+    <t>RdispNB</t>
+  </si>
+  <si>
+    <t>Cap./Nec. de financiación</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Importaciones </t>
+  </si>
+  <si>
+    <t>Var. de existencias</t>
+  </si>
+  <si>
+    <t>Adq. menos cesiones de objetos valiosos</t>
+  </si>
+  <si>
+    <t>Exportaciones</t>
+  </si>
+  <si>
+    <t>Impuestos sobre la prod. y las imp.</t>
+  </si>
+  <si>
+    <t>subvenciones rec. del RM</t>
+  </si>
+  <si>
+    <t>Rentas de la propiedad pag. a RM</t>
+  </si>
+  <si>
+    <t>Transferencias de capital pag. a RM</t>
+  </si>
+  <si>
+    <t>Rentas de la propiedad rec. de RM</t>
+  </si>
+  <si>
+    <t>Transferencias de capital rec. de RM</t>
+  </si>
+  <si>
+    <t>Impuestos corrientes</t>
+  </si>
+  <si>
+    <t>Impuestos corrientes pag. a RM</t>
+  </si>
+  <si>
+    <t>Impuestos corrientes rec. de RM</t>
+  </si>
+  <si>
+    <t>Cotiz. sociales netas</t>
+  </si>
+  <si>
+    <t>Cotiz. sociales netas pag. a RM</t>
+  </si>
+  <si>
+    <t>Cotiz. sociales netas rec. de RM</t>
+  </si>
+  <si>
+    <t>Prest. sociales dist. de las transf. sociales en especie</t>
+  </si>
+  <si>
+    <t>Prest. sociales dist. de las transf. sociales en especie pag. a RM</t>
+  </si>
+  <si>
+    <t>Prest. sociales dist. de las transf. sociales en especie rec. de RM</t>
+  </si>
+  <si>
+    <t>Otras transf. corrientes</t>
+  </si>
+  <si>
+    <t>Otras transf. corrientes pag. a RM</t>
+  </si>
+  <si>
+    <t>Otras transf. corrientes rec. de RM</t>
+  </si>
+  <si>
+    <t>Ajuste por la var. de los derechos por pensiones</t>
+  </si>
+  <si>
+    <t>Adq. menos cesiones de activos no prod.</t>
+  </si>
+  <si>
+    <t>Gasto en consumo final</t>
+  </si>
+  <si>
+    <t>Form. bruta de capital</t>
+  </si>
+  <si>
+    <t>Form. bruta de capital fijo</t>
+  </si>
+  <si>
+    <t>Cuenta de VPNdAyTC</t>
+  </si>
+  <si>
+    <t>Cuenta de adq. de activos no financieros</t>
+  </si>
+  <si>
+    <t>Cuenta de asign. de la renta primaria</t>
+  </si>
+  <si>
+    <t>Cuenta de distr. secundaria de la renta</t>
+  </si>
+  <si>
+    <t>grupos</t>
   </si>
 </sst>
 </file>
@@ -502,10 +613,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B48"/>
+  <dimension ref="A1:C48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C3" sqref="C2:C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -514,388 +625,532 @@
     <col min="2" max="2" width="40.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
       <c r="B17" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="C18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
       <c r="B19" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="C22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+      <c r="C23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+      <c r="C24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+      <c r="C25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+      <c r="C26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+      <c r="C27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+      <c r="C28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+      <c r="C29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+      <c r="C30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+      <c r="C31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+      <c r="C32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+      <c r="C33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+      <c r="C34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>34</v>
       </c>
       <c r="B35" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+      <c r="C36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+      <c r="C37">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+      <c r="C38">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+      <c r="C39">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>39</v>
       </c>
       <c r="B40" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C40">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+      <c r="C41">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>41</v>
       </c>
       <c r="B42" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>42</v>
       </c>
       <c r="B43" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+      <c r="C44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+      <c r="C45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+      <c r="C46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+      <c r="C47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>47</v>
       </c>
       <c r="B48" t="s">
         <v>47</v>
+      </c>
+      <c r="C48">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
no changes on order
</commit_message>
<xml_diff>
--- a/1.data/nodes_dict.xlsx
+++ b/1.data/nodes_dict.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4ba23d5b7de37717/Documentos/proyectos/03_GDP_visualization/1.data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="73" documentId="11_F25DC773A252ABDACC104888C19C6AFE5BDE58F4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9FB0C464-3031-4AAC-8D61-605A3EDA94A0}"/>
+  <xr:revisionPtr revIDLastSave="89" documentId="11_F25DC773A252ABDACC104888C19C6AFE5BDE58F4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0BA76EAE-C0C4-4BF8-B27C-7D8D1C9C3A24}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="106">
   <si>
     <t>names</t>
   </si>
@@ -282,13 +282,67 @@
     <t>Cuenta de adq. de activos no financieros</t>
   </si>
   <si>
-    <t>Cuenta de asign. de la renta primaria</t>
-  </si>
-  <si>
     <t>Cuenta de distr. secundaria de la renta</t>
   </si>
   <si>
     <t>grupos</t>
+  </si>
+  <si>
+    <t>FALSO2</t>
+  </si>
+  <si>
+    <t>FALSO3</t>
+  </si>
+  <si>
+    <t>FALSO4</t>
+  </si>
+  <si>
+    <t>FALSO5</t>
+  </si>
+  <si>
+    <t>FALSO6</t>
+  </si>
+  <si>
+    <t>FALSO7</t>
+  </si>
+  <si>
+    <t>FALSO8</t>
+  </si>
+  <si>
+    <t>FALSO9</t>
+  </si>
+  <si>
+    <t>FALSO10</t>
+  </si>
+  <si>
+    <t>FALSO11</t>
+  </si>
+  <si>
+    <t>FALSO12</t>
+  </si>
+  <si>
+    <t>FALSO13</t>
+  </si>
+  <si>
+    <t>FALSO14</t>
+  </si>
+  <si>
+    <t>FALSO15</t>
+  </si>
+  <si>
+    <t>FALSO16</t>
+  </si>
+  <si>
+    <t>FALSO17</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>FALSO1</t>
+  </si>
+  <si>
+    <t>Cuenta de asign. &lt;br&gt; de la renta primaria</t>
   </si>
 </sst>
 </file>
@@ -613,10 +667,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C48"/>
+  <dimension ref="A1:C65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C3" sqref="C2:C41"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -633,7 +687,7 @@
         <v>48</v>
       </c>
       <c r="C1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1125,7 +1179,7 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>85</v>
+        <v>105</v>
       </c>
       <c r="C46">
         <v>1</v>
@@ -1136,7 +1190,7 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C47">
         <v>1</v>
@@ -1151,6 +1205,190 @@
       </c>
       <c r="C48">
         <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>104</v>
+      </c>
+      <c r="C49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>87</v>
+      </c>
+      <c r="B50" t="s">
+        <v>103</v>
+      </c>
+      <c r="C50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>88</v>
+      </c>
+      <c r="B51" t="s">
+        <v>103</v>
+      </c>
+      <c r="C51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>89</v>
+      </c>
+      <c r="B52" t="s">
+        <v>103</v>
+      </c>
+      <c r="C52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>90</v>
+      </c>
+      <c r="B53" t="s">
+        <v>103</v>
+      </c>
+      <c r="C53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>91</v>
+      </c>
+      <c r="B54" t="s">
+        <v>103</v>
+      </c>
+      <c r="C54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>92</v>
+      </c>
+      <c r="B55" t="s">
+        <v>103</v>
+      </c>
+      <c r="C55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>93</v>
+      </c>
+      <c r="B56" t="s">
+        <v>103</v>
+      </c>
+      <c r="C56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>94</v>
+      </c>
+      <c r="B57" t="s">
+        <v>103</v>
+      </c>
+      <c r="C57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>95</v>
+      </c>
+      <c r="B58" t="s">
+        <v>103</v>
+      </c>
+      <c r="C58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>96</v>
+      </c>
+      <c r="B59" t="s">
+        <v>103</v>
+      </c>
+      <c r="C59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>97</v>
+      </c>
+      <c r="B60" t="s">
+        <v>103</v>
+      </c>
+      <c r="C60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>98</v>
+      </c>
+      <c r="B61" t="s">
+        <v>103</v>
+      </c>
+      <c r="C61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>99</v>
+      </c>
+      <c r="B62" t="s">
+        <v>103</v>
+      </c>
+      <c r="C62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>100</v>
+      </c>
+      <c r="B63" t="s">
+        <v>103</v>
+      </c>
+      <c r="C63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>101</v>
+      </c>
+      <c r="B64" t="s">
+        <v>103</v>
+      </c>
+      <c r="C64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>102</v>
+      </c>
+      <c r="B65" t="s">
+        <v>103</v>
+      </c>
+      <c r="C65">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
plotly en R, pero las subvenciones se cargan el flujo
</commit_message>
<xml_diff>
--- a/1.data/nodes_dict.xlsx
+++ b/1.data/nodes_dict.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4ba23d5b7de37717/Documentos/proyectos/03_GDP_visualization/1.data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="125" documentId="11_F25DC773A252ABDACC104888C19C6AFE5BDE58F4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1328084D-96CF-4A69-B13B-2876B4CAD8BF}"/>
+  <xr:revisionPtr revIDLastSave="240" documentId="11_F25DC773A252ABDACC104888C19C6AFE5BDE58F4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F79FB954-8B09-4685-AAD2-176E61BA813C}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3240" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="92">
   <si>
     <t>names</t>
   </si>
@@ -288,60 +288,6 @@
     <t>grupos</t>
   </si>
   <si>
-    <t>FALSO2</t>
-  </si>
-  <si>
-    <t>FALSO3</t>
-  </si>
-  <si>
-    <t>FALSO4</t>
-  </si>
-  <si>
-    <t>FALSO5</t>
-  </si>
-  <si>
-    <t>FALSO6</t>
-  </si>
-  <si>
-    <t>FALSO7</t>
-  </si>
-  <si>
-    <t>FALSO8</t>
-  </si>
-  <si>
-    <t>FALSO9</t>
-  </si>
-  <si>
-    <t>FALSO10</t>
-  </si>
-  <si>
-    <t>FALSO11</t>
-  </si>
-  <si>
-    <t>FALSO12</t>
-  </si>
-  <si>
-    <t>FALSO13</t>
-  </si>
-  <si>
-    <t>FALSO14</t>
-  </si>
-  <si>
-    <t>FALSO15</t>
-  </si>
-  <si>
-    <t>FALSO16</t>
-  </si>
-  <si>
-    <t>FALSO17</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>FALSO1</t>
-  </si>
-  <si>
     <t>a</t>
   </si>
   <si>
@@ -349,6 +295,12 @@
   </si>
   <si>
     <t>Cuenta de asign. de la renta primaria</t>
+  </si>
+  <si>
+    <t>x_pos</t>
+  </si>
+  <si>
+    <t>y_pos</t>
   </si>
 </sst>
 </file>
@@ -673,10 +625,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C65"/>
+  <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="B63" sqref="B63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -685,7 +637,7 @@
     <col min="2" max="2" width="40.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -695,8 +647,14 @@
       <c r="C1" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -704,10 +662,16 @@
         <v>52</v>
       </c>
       <c r="C2" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -717,8 +681,14 @@
       <c r="C3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3">
+        <v>12</v>
+      </c>
+      <c r="E3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -726,10 +696,16 @@
         <v>51</v>
       </c>
       <c r="C4" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -737,10 +713,16 @@
         <v>53</v>
       </c>
       <c r="C5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+      <c r="D5">
+        <v>5</v>
+      </c>
+      <c r="E5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -748,10 +730,16 @@
         <v>54</v>
       </c>
       <c r="C6" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+      <c r="D6">
+        <v>7</v>
+      </c>
+      <c r="E6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -761,8 +749,14 @@
       <c r="C7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7">
+        <v>9</v>
+      </c>
+      <c r="E7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -772,8 +766,14 @@
       <c r="C8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8">
+        <v>10</v>
+      </c>
+      <c r="E8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -783,8 +783,14 @@
       <c r="C9" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9">
+        <v>14</v>
+      </c>
+      <c r="E9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -794,8 +800,14 @@
       <c r="C10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10">
+        <v>17</v>
+      </c>
+      <c r="E10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -805,8 +817,14 @@
       <c r="C11" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11">
+        <v>15</v>
+      </c>
+      <c r="E11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -816,8 +834,14 @@
       <c r="C12" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12">
+        <v>15</v>
+      </c>
+      <c r="E12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -827,8 +851,14 @@
       <c r="C13" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13">
+        <v>15</v>
+      </c>
+      <c r="E13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -838,8 +868,14 @@
       <c r="C14" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14">
+        <v>15</v>
+      </c>
+      <c r="E14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -847,10 +883,16 @@
         <v>50</v>
       </c>
       <c r="C15" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+      <c r="D15">
+        <v>3</v>
+      </c>
+      <c r="E15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -858,10 +900,16 @@
         <v>60</v>
       </c>
       <c r="C16" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+      <c r="D16">
+        <v>3</v>
+      </c>
+      <c r="E16">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -871,8 +919,14 @@
       <c r="C17" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17">
+        <v>5</v>
+      </c>
+      <c r="E17">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -882,8 +936,14 @@
       <c r="C18" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -893,8 +953,14 @@
       <c r="C19" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19">
+        <v>3</v>
+      </c>
+      <c r="E19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -904,8 +970,14 @@
       <c r="C20" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20">
+        <v>5</v>
+      </c>
+      <c r="E20">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -915,8 +987,14 @@
       <c r="C21" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21">
+        <v>2</v>
+      </c>
+      <c r="E21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -926,8 +1004,14 @@
       <c r="C22" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D22">
+        <v>5</v>
+      </c>
+      <c r="E22">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -937,8 +1021,14 @@
       <c r="C23" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D23">
+        <v>7</v>
+      </c>
+      <c r="E23">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -948,8 +1038,14 @@
       <c r="C24" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D24">
+        <v>4</v>
+      </c>
+      <c r="E24">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -959,8 +1055,14 @@
       <c r="C25" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D25">
+        <v>5</v>
+      </c>
+      <c r="E25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -970,8 +1072,14 @@
       <c r="C26" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D26">
+        <v>7</v>
+      </c>
+      <c r="E26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -981,8 +1089,14 @@
       <c r="C27" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D27">
+        <v>4</v>
+      </c>
+      <c r="E27">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -992,8 +1106,14 @@
       <c r="C28" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D28">
+        <v>5</v>
+      </c>
+      <c r="E28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -1003,8 +1123,14 @@
       <c r="C29" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D29">
+        <v>7</v>
+      </c>
+      <c r="E29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -1014,8 +1140,14 @@
       <c r="C30" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D30">
+        <v>4</v>
+      </c>
+      <c r="E30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -1025,8 +1157,14 @@
       <c r="C31" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D31">
+        <v>5</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -1036,8 +1174,14 @@
       <c r="C32" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D32">
+        <v>7</v>
+      </c>
+      <c r="E32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -1047,8 +1191,14 @@
       <c r="C33" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D33">
+        <v>4</v>
+      </c>
+      <c r="E33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -1058,8 +1208,14 @@
       <c r="C34" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D34">
+        <v>7</v>
+      </c>
+      <c r="E34">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -1069,8 +1225,14 @@
       <c r="C35" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D35">
+        <v>12</v>
+      </c>
+      <c r="E35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -1080,8 +1242,14 @@
       <c r="C36" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D36">
+        <v>13</v>
+      </c>
+      <c r="E36">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -1091,8 +1259,14 @@
       <c r="C37" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D37">
+        <v>10</v>
+      </c>
+      <c r="E37">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>37</v>
       </c>
@@ -1102,8 +1276,14 @@
       <c r="C38" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D38">
+        <v>12</v>
+      </c>
+      <c r="E38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>38</v>
       </c>
@@ -1113,8 +1293,14 @@
       <c r="C39" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D39">
+        <v>9</v>
+      </c>
+      <c r="E39">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>39</v>
       </c>
@@ -1124,8 +1310,14 @@
       <c r="C40" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D40">
+        <v>10</v>
+      </c>
+      <c r="E40">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>40</v>
       </c>
@@ -1135,8 +1327,14 @@
       <c r="C41" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D41">
+        <v>14</v>
+      </c>
+      <c r="E41">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>41</v>
       </c>
@@ -1144,10 +1342,16 @@
         <v>41</v>
       </c>
       <c r="C42" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+      <c r="D42">
+        <v>16</v>
+      </c>
+      <c r="E42">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>42</v>
       </c>
@@ -1155,10 +1359,16 @@
         <v>42</v>
       </c>
       <c r="C43" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+      <c r="D43">
+        <v>2</v>
+      </c>
+      <c r="E43">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>43</v>
       </c>
@@ -1166,10 +1376,16 @@
         <v>83</v>
       </c>
       <c r="C44" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+      <c r="D44">
+        <v>11</v>
+      </c>
+      <c r="E44">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>44</v>
       </c>
@@ -1177,21 +1393,33 @@
         <v>84</v>
       </c>
       <c r="C45" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+      <c r="D45">
+        <v>13</v>
+      </c>
+      <c r="E45">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>107</v>
+        <v>89</v>
       </c>
       <c r="C46" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+      <c r="D46">
+        <v>4</v>
+      </c>
+      <c r="E46">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>46</v>
       </c>
@@ -1199,10 +1427,16 @@
         <v>85</v>
       </c>
       <c r="C47" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+      <c r="D47">
+        <v>6</v>
+      </c>
+      <c r="E47">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>47</v>
       </c>
@@ -1210,191 +1444,13 @@
         <v>47</v>
       </c>
       <c r="C48" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>104</v>
-      </c>
-      <c r="C49" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
         <v>87</v>
       </c>
-      <c r="B50" t="s">
-        <v>103</v>
-      </c>
-      <c r="C50" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>88</v>
-      </c>
-      <c r="B51" t="s">
-        <v>103</v>
-      </c>
-      <c r="C51" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>89</v>
-      </c>
-      <c r="B52" t="s">
-        <v>103</v>
-      </c>
-      <c r="C52" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>90</v>
-      </c>
-      <c r="B53" t="s">
-        <v>103</v>
-      </c>
-      <c r="C53" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>91</v>
-      </c>
-      <c r="B54" t="s">
-        <v>103</v>
-      </c>
-      <c r="C54" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>92</v>
-      </c>
-      <c r="B55" t="s">
-        <v>103</v>
-      </c>
-      <c r="C55" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>93</v>
-      </c>
-      <c r="B56" t="s">
-        <v>103</v>
-      </c>
-      <c r="C56" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>94</v>
-      </c>
-      <c r="B57" t="s">
-        <v>103</v>
-      </c>
-      <c r="C57" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>95</v>
-      </c>
-      <c r="B58" t="s">
-        <v>103</v>
-      </c>
-      <c r="C58" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>96</v>
-      </c>
-      <c r="B59" t="s">
-        <v>103</v>
-      </c>
-      <c r="C59" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>97</v>
-      </c>
-      <c r="B60" t="s">
-        <v>103</v>
-      </c>
-      <c r="C60" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>98</v>
-      </c>
-      <c r="B61" t="s">
-        <v>103</v>
-      </c>
-      <c r="C61" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>99</v>
-      </c>
-      <c r="B62" t="s">
-        <v>103</v>
-      </c>
-      <c r="C62" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>100</v>
-      </c>
-      <c r="B63" t="s">
-        <v>103</v>
-      </c>
-      <c r="C63" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>101</v>
-      </c>
-      <c r="B64" t="s">
-        <v>103</v>
-      </c>
-      <c r="C64" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>102</v>
-      </c>
-      <c r="B65" t="s">
-        <v>103</v>
-      </c>
-      <c r="C65" t="s">
-        <v>102</v>
+      <c r="D48">
+        <v>8</v>
+      </c>
+      <c r="E48">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>